<commit_message>
initial commit to debug
</commit_message>
<xml_diff>
--- a/Input/Einkauf Kiosk  01.11.23.xlsx
+++ b/Input/Einkauf Kiosk  01.11.23.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4920E7-1C17-487E-98DC-AE5DFCE3C540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B0C0A-E41D-4BC1-AC6C-D74713FCFA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
   </bookViews>
   <sheets>
-    <sheet name="KinoKiosk Angebot 2023" sheetId="1" r:id="rId1"/>
-    <sheet name="Theater Bar" sheetId="2" r:id="rId2"/>
+    <sheet name="Angebot" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="81">
   <si>
     <t>Schüwo</t>
   </si>
@@ -120,49 +119,7 @@
     <t>Eistee</t>
   </si>
   <si>
-    <t>Campari</t>
-  </si>
-  <si>
-    <t>Gin Tonic</t>
-  </si>
-  <si>
-    <t>Gazosa</t>
-  </si>
-  <si>
-    <t>Cola</t>
-  </si>
-  <si>
-    <t>Mineral</t>
-  </si>
-  <si>
-    <t>Kaffee</t>
-  </si>
-  <si>
     <t>Bier</t>
-  </si>
-  <si>
-    <t>Apero Spritz</t>
-  </si>
-  <si>
-    <t>Gespritzer Weisswein</t>
-  </si>
-  <si>
-    <t>Hugo</t>
-  </si>
-  <si>
-    <t>Whiskey Cola</t>
-  </si>
-  <si>
-    <t>Wein</t>
-  </si>
-  <si>
-    <t>Getränk</t>
-  </si>
-  <si>
-    <t>Preis</t>
-  </si>
-  <si>
-    <t>Preis alt</t>
   </si>
   <si>
     <t>30g</t>
@@ -864,18 +821,6 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{72CB00EF-10E8-41AE-8833-34C494F4A79D}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13" xr:uid="{72CB00EF-10E8-41AE-8833-34C494F4A79D}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{13AABF72-04A9-4F5D-B788-824B43C06F21}" name="Getränk"/>
-    <tableColumn id="2" xr3:uid="{5407815B-DC16-417D-A8B1-134E20E0D9EC}" name="Preis"/>
-    <tableColumn id="3" xr3:uid="{8A1241EB-4EA9-4825-86AB-CF7104EBA61B}" name="Preis alt"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1178,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677428D-B810-4F63-BFBD-79DB0D9DB708}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,16 +1144,16 @@
         <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>21</v>
@@ -1217,24 +1162,24 @@
         <v>22</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5">
         <v>1.38</v>
@@ -1254,16 +1199,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C3" s="5">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E3" s="5">
         <v>1.65</v>
@@ -1340,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -1350,7 +1295,7 @@
         <v>0.15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G6" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1364,10 +1309,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5">
         <v>4</v>
@@ -1377,7 +1322,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G7" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1400,7 +1345,7 @@
         <v>4.5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E8" s="5">
         <v>1.55</v>
@@ -1429,7 +1374,7 @@
         <v>4.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5">
         <v>1.55</v>
@@ -1458,7 +1403,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E10" s="5">
         <v>0.97</v>
@@ -1487,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5">
         <v>0.97</v>
@@ -1520,7 +1465,7 @@
         <v>0.3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G12" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1537,13 +1482,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E13" s="5">
         <v>1.1499999999999999</v>
@@ -1566,13 +1511,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5">
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5">
         <v>1.1499999999999999</v>
@@ -1601,7 +1546,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5">
         <v>1.44</v>
@@ -1630,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5">
         <v>1.1200000000000001</v>
@@ -1659,7 +1604,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5">
         <v>1.44</v>
@@ -1688,7 +1633,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E18" s="5">
         <v>1.44</v>
@@ -1717,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E19" s="6">
         <v>1.03</v>
@@ -1746,7 +1691,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E20" s="7">
         <v>1.95</v>
@@ -1766,16 +1711,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5">
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5">
         <v>2.2000000000000002</v>
@@ -1795,22 +1740,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5">
         <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E22" s="5">
         <v>0.4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G22" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1833,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E23" s="7">
         <v>4.17</v>
@@ -1862,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E24" s="5">
         <v>1.06</v>
@@ -1891,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E25" s="5">
         <v>1.06</v>
@@ -1920,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E26" s="5">
         <v>1.06</v>
@@ -1949,7 +1894,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E27" s="5">
         <v>1.06</v>
@@ -1969,16 +1914,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C28" s="6">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E28" s="6">
         <v>0.99</v>
@@ -1998,16 +1943,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E29" s="5">
         <v>2.2999999999999998</v>
@@ -2027,16 +1972,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5">
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E30" s="5">
         <v>2.2999999999999998</v>
@@ -2056,16 +2001,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C31" s="5">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E31" s="5">
         <v>2.2999999999999998</v>
@@ -2085,16 +2030,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C32" s="5">
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E32" s="5">
         <v>2.2999999999999998</v>
@@ -2114,16 +2059,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E33" s="5">
         <v>2.2999999999999998</v>
@@ -2143,22 +2088,22 @@
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C34" s="5">
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E34" s="17">
         <v>3</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G34" s="17">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -2172,22 +2117,22 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C35" s="5">
         <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E35" s="17">
         <v>3</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G35" s="17">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -2201,22 +2146,22 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C36" s="5">
         <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E36" s="17">
         <v>3</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G36" s="17">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -2230,22 +2175,22 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C37" s="5">
         <v>4</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E37" s="17">
         <v>3</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G37" s="17">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -2259,22 +2204,22 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C38" s="5">
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E38" s="17">
         <v>3</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G38" s="17">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -2294,137 +2239,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B683F7-C2A7-4618-8D69-650AF98B84B2}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>